<commit_message>
Refactor code to improve peak detection algorithm
</commit_message>
<xml_diff>
--- a/Resultats exp bag_couverts/Resultats exp bag_couverts/Tableau récapitulatif - new algo.xlsx
+++ b/Resultats exp bag_couverts/Resultats exp bag_couverts/Tableau récapitulatif - new algo.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12696" tabRatio="600" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="11625" tabRatio="600" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Menu" sheetId="1" state="visible" r:id="rId1"/>
@@ -585,19 +585,19 @@
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="14.25"/>
   <cols>
     <col width="11.6640625" customWidth="1" style="4" min="1" max="1"/>
-    <col width="14.109375" customWidth="1" style="4" min="2" max="2"/>
+    <col width="14.1328125" customWidth="1" style="4" min="2" max="2"/>
     <col width="47.33203125" customWidth="1" style="4" min="3" max="3"/>
-    <col width="20.109375" customWidth="1" style="4" min="4" max="4"/>
-    <col width="14.44140625" customWidth="1" style="4" min="5" max="5"/>
+    <col width="20.1328125" customWidth="1" style="4" min="4" max="4"/>
+    <col width="14.46484375" customWidth="1" style="4" min="5" max="5"/>
     <col width="13.6640625" customWidth="1" style="4" min="6" max="9"/>
     <col width="11" customWidth="1" style="4" min="10" max="10"/>
     <col width="36.6640625" customWidth="1" style="4" min="11" max="11"/>
   </cols>
   <sheetData>
-    <row r="1" ht="31.95" customHeight="1">
+    <row r="1" ht="32" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Date</t>
@@ -654,7 +654,7 @@
         </is>
       </c>
     </row>
-    <row r="2" ht="31.95" customHeight="1">
+    <row r="2" ht="32" customHeight="1">
       <c r="A2" s="2" t="n">
         <v>45439</v>
       </c>
@@ -698,7 +698,7 @@
         </is>
       </c>
     </row>
-    <row r="3" ht="31.95" customHeight="1">
+    <row r="3" ht="32" customHeight="1">
       <c r="A3" s="2" t="n">
         <v>45439</v>
       </c>
@@ -742,7 +742,7 @@
         </is>
       </c>
     </row>
-    <row r="4" ht="31.95" customHeight="1">
+    <row r="4" ht="32" customHeight="1">
       <c r="A4" s="2" t="n">
         <v>45439</v>
       </c>
@@ -786,7 +786,7 @@
         </is>
       </c>
     </row>
-    <row r="5" ht="31.95" customHeight="1">
+    <row r="5" ht="32" customHeight="1">
       <c r="A5" s="2" t="n">
         <v>45439</v>
       </c>
@@ -830,7 +830,7 @@
         </is>
       </c>
     </row>
-    <row r="6" ht="31.95" customHeight="1">
+    <row r="6" ht="32" customHeight="1">
       <c r="A6" s="2" t="n">
         <v>45439</v>
       </c>
@@ -874,7 +874,7 @@
         </is>
       </c>
     </row>
-    <row r="7" ht="31.95" customHeight="1">
+    <row r="7" ht="32" customHeight="1">
       <c r="A7" s="2" t="n">
         <v>45439</v>
       </c>
@@ -918,7 +918,7 @@
         </is>
       </c>
     </row>
-    <row r="8" ht="31.95" customHeight="1">
+    <row r="8" ht="32" customHeight="1">
       <c r="A8" s="2" t="n">
         <v>45440</v>
       </c>
@@ -962,7 +962,7 @@
         </is>
       </c>
     </row>
-    <row r="9" ht="31.95" customHeight="1">
+    <row r="9" ht="32" customHeight="1">
       <c r="A9" s="2" t="n">
         <v>45440</v>
       </c>
@@ -1006,7 +1006,7 @@
         </is>
       </c>
     </row>
-    <row r="10" ht="31.95" customHeight="1">
+    <row r="10" ht="32" customHeight="1">
       <c r="A10" s="2" t="n">
         <v>45440</v>
       </c>
@@ -1050,7 +1050,7 @@
         </is>
       </c>
     </row>
-    <row r="11" ht="31.95" customHeight="1">
+    <row r="11" ht="32" customHeight="1">
       <c r="A11" s="2" t="n">
         <v>45440</v>
       </c>
@@ -1094,7 +1094,7 @@
         </is>
       </c>
     </row>
-    <row r="12" ht="31.95" customHeight="1">
+    <row r="12" ht="32" customHeight="1">
       <c r="A12" s="2" t="n">
         <v>45440</v>
       </c>
@@ -1158,7 +1158,7 @@
       <selection activeCell="N25" sqref="N25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
@@ -2246,12 +2246,12 @@
   <dimension ref="A1:U32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="S24" sqref="S24"/>
+      <selection activeCell="Q11" sqref="Q11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
   <cols>
-    <col width="39.77734375" customWidth="1" min="20" max="20"/>
+    <col width="39.796875" customWidth="1" min="20" max="20"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>

<commit_message>
detect more peaks and correct the weight
</commit_message>
<xml_diff>
--- a/Resultats exp bag_couverts/Resultats exp bag_couverts/Tableau récapitulatif - new algo.xlsx
+++ b/Resultats exp bag_couverts/Resultats exp bag_couverts/Tableau récapitulatif - new algo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abarb\Documents\travail\stage et4\travail\codePlateau\Resultats exp bag_couverts\Resultats exp bag_couverts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{925BCB33-90B5-4C3C-96F1-7B96D9A1336E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A72450A-11C7-4A8C-AF00-2CEE94F123A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="11625" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1250,7 +1250,7 @@
   <dimension ref="A1:J31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N25" sqref="N25"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2257,7 +2257,7 @@
   <dimension ref="A1:U32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="V9" sqref="V9"/>
+      <selection activeCell="A8" sqref="A8:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2362,31 +2362,31 @@
         <v>1</v>
       </c>
       <c r="K2" s="6">
-        <v>292.42399999999998</v>
+        <v>290.60400000000004</v>
       </c>
       <c r="L2" s="6">
         <v>199</v>
       </c>
       <c r="M2" s="6">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="N2" s="6">
-        <v>161.114</v>
+        <v>125.94099999999997</v>
       </c>
       <c r="O2" s="6">
-        <v>9.4770000000000003</v>
+        <v>5.476</v>
       </c>
       <c r="P2" s="6">
-        <v>27.087</v>
+        <v>20.214999999999975</v>
       </c>
       <c r="Q2" s="6">
-        <v>1.4159999999999999</v>
+        <v>0.40399999999999636</v>
       </c>
       <c r="R2" s="6">
-        <v>55.1</v>
+        <v>43.3</v>
       </c>
       <c r="S2" s="6">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="T2" s="6" t="s">
         <v>36</v>
@@ -2427,31 +2427,31 @@
         <v>1</v>
       </c>
       <c r="K3" s="6">
-        <v>173.88499999999999</v>
+        <v>172.87400000000002</v>
       </c>
       <c r="L3" s="6">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="M3" s="6">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="N3" s="6">
-        <v>80.876000000000005</v>
+        <v>63.284999999999968</v>
       </c>
       <c r="O3" s="6">
-        <v>5.3920000000000003</v>
+        <v>4.8680000000000003</v>
       </c>
       <c r="P3" s="6">
-        <v>8.4939999999999998</v>
+        <v>7.0779999999999745</v>
       </c>
       <c r="Q3" s="6">
-        <v>1.214</v>
+        <v>0.20100000000002183</v>
       </c>
       <c r="R3" s="6">
-        <v>46.5</v>
+        <v>36.6</v>
       </c>
       <c r="S3" s="6">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="T3" s="6" t="s">
         <v>37</v>
@@ -2539,31 +2539,31 @@
         <v>2</v>
       </c>
       <c r="K5" s="6">
-        <v>273.42099999999999</v>
+        <v>272.40999999999997</v>
       </c>
       <c r="L5" s="6">
         <v>141</v>
       </c>
       <c r="M5" s="6">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="N5" s="6">
-        <v>142.21700000000001</v>
+        <v>92.68900000000005</v>
       </c>
       <c r="O5" s="6">
-        <v>4.5880000000000001</v>
+        <v>2.5750000000000002</v>
       </c>
       <c r="P5" s="6">
-        <v>17.187999999999999</v>
+        <v>8.8980000000000246</v>
       </c>
       <c r="Q5" s="6">
-        <v>1.01</v>
+        <v>0.20199999999999818</v>
       </c>
       <c r="R5" s="6">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="S5" s="6">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="T5" s="6" t="s">
         <v>38</v>
@@ -2604,31 +2604,31 @@
         <v>2</v>
       </c>
       <c r="K6" s="6">
-        <v>229.476</v>
+        <v>226.44399999999996</v>
       </c>
       <c r="L6" s="6">
         <v>169</v>
       </c>
       <c r="M6" s="6">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="N6" s="6">
-        <v>133.441</v>
+        <v>90.380000000000223</v>
       </c>
       <c r="O6" s="6">
-        <v>8.8960000000000008</v>
+        <v>4.7569999999999997</v>
       </c>
       <c r="P6" s="6">
-        <v>20.625</v>
+        <v>8.4920000000000755</v>
       </c>
       <c r="Q6" s="6">
-        <v>4.0430000000000001</v>
+        <v>0.20299999999997453</v>
       </c>
       <c r="R6" s="6">
-        <v>58.2</v>
+        <v>39.9</v>
       </c>
       <c r="S6" s="6">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="T6" s="6" t="s">
         <v>39</v>
@@ -2669,31 +2669,31 @@
         <v>2</v>
       </c>
       <c r="K7" s="6">
-        <v>498.46100000000001</v>
+        <v>490.779</v>
       </c>
       <c r="L7" s="6">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="M7" s="6">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="N7" s="6">
-        <v>165.18</v>
+        <v>116.24700000000053</v>
       </c>
       <c r="O7" s="6">
-        <v>6.3529999999999998</v>
+        <v>5.0540000000000003</v>
       </c>
       <c r="P7" s="6">
-        <v>15.569000000000001</v>
+        <v>14.154999999999973</v>
       </c>
       <c r="Q7" s="6">
-        <v>1.2130000000000001</v>
+        <v>0.20199999999999818</v>
       </c>
       <c r="R7" s="6">
-        <v>33.1</v>
+        <v>23.7</v>
       </c>
       <c r="S7" s="6">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="T7" s="6" t="s">
         <v>40</v>
@@ -2734,31 +2734,31 @@
         <v>1</v>
       </c>
       <c r="K8" s="6">
-        <v>289.971</v>
+        <v>288.45399999999995</v>
       </c>
       <c r="L8" s="6">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="M8" s="6">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="N8" s="6">
-        <v>139.458</v>
+        <v>87.703999999999922</v>
       </c>
       <c r="O8" s="6">
-        <v>5.8109999999999999</v>
+        <v>2.7410000000000001</v>
       </c>
       <c r="P8" s="6">
-        <v>14.076000000000001</v>
+        <v>8.4459999999999695</v>
       </c>
       <c r="Q8" s="6">
-        <v>1.7310000000000001</v>
+        <v>0.21600000000000819</v>
       </c>
       <c r="R8" s="6">
-        <v>48.1</v>
+        <v>30.4</v>
       </c>
       <c r="S8" s="6">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="T8" s="6" t="s">
         <v>41</v>
@@ -2799,31 +2799,31 @@
         <v>1</v>
       </c>
       <c r="K9" s="6">
-        <v>227.38300000000001</v>
+        <v>193.71000000000004</v>
       </c>
       <c r="L9" s="6">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="M9" s="6">
+        <v>22</v>
+      </c>
+      <c r="N9" s="6">
+        <v>51.976999999999748</v>
+      </c>
+      <c r="O9" s="6">
+        <v>2.5990000000000002</v>
+      </c>
+      <c r="P9" s="6">
+        <v>3.8979999999999109</v>
+      </c>
+      <c r="Q9" s="6">
+        <v>0.21699999999998454</v>
+      </c>
+      <c r="R9" s="6">
+        <v>26.8</v>
+      </c>
+      <c r="S9" s="6">
         <v>20</v>
-      </c>
-      <c r="N9" s="6">
-        <v>85.54</v>
-      </c>
-      <c r="O9" s="6">
-        <v>4.2770000000000001</v>
-      </c>
-      <c r="P9" s="6">
-        <v>14.726000000000001</v>
-      </c>
-      <c r="Q9" s="6">
-        <v>1.732</v>
-      </c>
-      <c r="R9" s="6">
-        <v>37.6</v>
-      </c>
-      <c r="S9" s="6">
-        <v>15</v>
       </c>
       <c r="T9" s="6" t="s">
         <v>42</v>
@@ -2864,31 +2864,31 @@
         <v>1</v>
       </c>
       <c r="K10" s="6">
-        <v>62.581000000000003</v>
+        <v>51.322000000000003</v>
       </c>
       <c r="L10" s="6">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="M10" s="6">
+        <v>10</v>
+      </c>
+      <c r="N10" s="6">
+        <v>28.586000000000013</v>
+      </c>
+      <c r="O10" s="6">
+        <v>3.573</v>
+      </c>
+      <c r="P10" s="6">
+        <v>10.394999999999982</v>
+      </c>
+      <c r="Q10" s="6">
+        <v>0.43299999999999272</v>
+      </c>
+      <c r="R10" s="6">
+        <v>55.7</v>
+      </c>
+      <c r="S10" s="6">
         <v>8</v>
-      </c>
-      <c r="N10" s="6">
-        <v>46.771999999999998</v>
-      </c>
-      <c r="O10" s="6">
-        <v>5.8460000000000001</v>
-      </c>
-      <c r="P10" s="6">
-        <v>14.941000000000001</v>
-      </c>
-      <c r="Q10" s="6">
-        <v>1.5149999999999999</v>
-      </c>
-      <c r="R10" s="6">
-        <v>74.7</v>
-      </c>
-      <c r="S10" s="6">
-        <v>5</v>
       </c>
       <c r="T10" s="6" t="s">
         <v>43</v>
@@ -2929,31 +2929,31 @@
         <v>2</v>
       </c>
       <c r="K11" s="6">
-        <v>281.52499999999998</v>
+        <v>262.46799999999996</v>
       </c>
       <c r="L11" s="6">
-        <v>132</v>
+        <v>146</v>
       </c>
       <c r="M11" s="6">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="N11" s="6">
-        <v>152.244</v>
+        <v>106.54500000000004</v>
       </c>
       <c r="O11" s="6">
-        <v>5.8559999999999999</v>
+        <v>4.843</v>
       </c>
       <c r="P11" s="6">
-        <v>19.274000000000001</v>
+        <v>8.4449999999999932</v>
       </c>
       <c r="Q11" s="6">
-        <v>0.65</v>
+        <v>0.21600000000000819</v>
       </c>
       <c r="R11" s="6">
-        <v>54.1</v>
+        <v>40.6</v>
       </c>
       <c r="S11" s="6">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="T11" s="6" t="s">
         <v>44</v>
@@ -2994,31 +2994,31 @@
         <v>2</v>
       </c>
       <c r="K12" s="6">
-        <v>221.75299999999999</v>
+        <v>214.28099999999995</v>
       </c>
       <c r="L12" s="6">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="M12" s="6">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="N12" s="6">
-        <v>140.11000000000001</v>
+        <v>81.538000000000238</v>
       </c>
       <c r="O12" s="6">
-        <v>7.3739999999999997</v>
+        <v>3.5449999999999999</v>
       </c>
       <c r="P12" s="6">
-        <v>24.687000000000001</v>
+        <v>6.7119999999999891</v>
       </c>
       <c r="Q12" s="6">
-        <v>2.3820000000000001</v>
+        <v>0.64999999999997726</v>
       </c>
       <c r="R12" s="6">
-        <v>63.2</v>
+        <v>38.1</v>
       </c>
       <c r="S12" s="6">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="T12" s="6" t="s">
         <v>45</v>
@@ -3059,31 +3059,31 @@
         <v>2</v>
       </c>
       <c r="K13" s="6">
-        <v>447.947</v>
+        <v>395.53899999999999</v>
       </c>
       <c r="L13" s="6">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="M13" s="6">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="N13" s="6">
-        <v>258.35199999999998</v>
+        <v>197.06600000000094</v>
       </c>
       <c r="O13" s="6">
-        <v>8.3339999999999996</v>
+        <v>7.2990000000000004</v>
       </c>
       <c r="P13" s="6">
-        <v>26.419</v>
+        <v>14.076000000000022</v>
       </c>
       <c r="Q13" s="6">
-        <v>1.0840000000000001</v>
+        <v>0.43299999999999272</v>
       </c>
       <c r="R13" s="6">
-        <v>57.7</v>
+        <v>49.8</v>
       </c>
       <c r="S13" s="6">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="T13" s="6" t="s">
         <v>46</v>
@@ -3124,31 +3124,31 @@
         <v>3</v>
       </c>
       <c r="K14" s="6">
-        <v>264.74299999999999</v>
+        <v>250.34200000000001</v>
       </c>
       <c r="L14" s="6">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="M14" s="6">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="N14" s="6">
-        <v>76.984999999999999</v>
+        <v>46.778999999999911</v>
       </c>
       <c r="O14" s="6">
-        <v>2.851</v>
+        <v>2.2280000000000002</v>
       </c>
       <c r="P14" s="6">
-        <v>5.1980000000000004</v>
+        <v>3.6819999999999595</v>
       </c>
       <c r="Q14" s="6">
-        <v>1.298</v>
+        <v>0.21600000000000819</v>
       </c>
       <c r="R14" s="6">
-        <v>29.1</v>
+        <v>18.7</v>
       </c>
       <c r="S14" s="6">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="T14" s="6" t="s">
         <v>47</v>
@@ -3189,31 +3189,31 @@
         <v>3</v>
       </c>
       <c r="K15" s="6">
-        <v>214.714</v>
+        <v>214.71500000000003</v>
       </c>
       <c r="L15" s="6">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="M15" s="6">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="N15" s="6">
-        <v>131.12100000000001</v>
+        <v>90.717999999999734</v>
       </c>
       <c r="O15" s="6">
-        <v>6.9009999999999998</v>
+        <v>5.04</v>
       </c>
       <c r="P15" s="6">
-        <v>12.343999999999999</v>
+        <v>9.3120000000000118</v>
       </c>
       <c r="Q15" s="6">
-        <v>3.4649999999999999</v>
+        <v>0.41699999999991633</v>
       </c>
       <c r="R15" s="6">
-        <v>61.1</v>
+        <v>42.3</v>
       </c>
       <c r="S15" s="6">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="T15" s="6" t="s">
         <v>48</v>
@@ -3254,31 +3254,31 @@
         <v>3</v>
       </c>
       <c r="K16" s="6">
-        <v>456.28399999999999</v>
+        <v>455.30900000000008</v>
       </c>
       <c r="L16" s="6">
         <v>178</v>
       </c>
       <c r="M16" s="6">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="N16" s="6">
-        <v>254.239</v>
+        <v>204.19700000000046</v>
       </c>
       <c r="O16" s="6">
-        <v>8.2010000000000005</v>
+        <v>7.2930000000000001</v>
       </c>
       <c r="P16" s="6">
-        <v>25.555</v>
+        <v>13.426000000000158</v>
       </c>
       <c r="Q16" s="6">
-        <v>2.165</v>
+        <v>0.21600000000000819</v>
       </c>
       <c r="R16" s="6">
-        <v>55.7</v>
+        <v>44.8</v>
       </c>
       <c r="S16" s="6">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="T16" s="6" t="s">
         <v>49</v>
@@ -3319,31 +3319,31 @@
         <v>4</v>
       </c>
       <c r="K17" s="6">
-        <v>292.46199999999999</v>
+        <v>291.48700000000002</v>
       </c>
       <c r="L17" s="6">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="M17" s="6">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="N17" s="6">
-        <v>121.587</v>
+        <v>91.391999999999882</v>
       </c>
       <c r="O17" s="6">
-        <v>3.8</v>
+        <v>3.2639999999999998</v>
       </c>
       <c r="P17" s="6">
-        <v>10.61</v>
+        <v>10.394999999999982</v>
       </c>
       <c r="Q17" s="6">
-        <v>1.0820000000000001</v>
+        <v>0.21699999999998454</v>
       </c>
       <c r="R17" s="6">
-        <v>41.6</v>
+        <v>31.4</v>
       </c>
       <c r="S17" s="6">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="T17" s="6" t="s">
         <v>50</v>
@@ -3384,31 +3384,31 @@
         <v>4</v>
       </c>
       <c r="K18" s="6">
-        <v>237.995</v>
+        <v>234.20500000000004</v>
       </c>
       <c r="L18" s="6">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="M18" s="6">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="N18" s="6">
-        <v>113.04300000000001</v>
+        <v>84.456000000000017</v>
       </c>
       <c r="O18" s="6">
-        <v>7.0650000000000004</v>
+        <v>6.0330000000000004</v>
       </c>
       <c r="P18" s="6">
-        <v>16.675000000000001</v>
+        <v>9.3129999999999882</v>
       </c>
       <c r="Q18" s="6">
-        <v>1.732</v>
+        <v>0.21699999999998454</v>
       </c>
       <c r="R18" s="6">
-        <v>47.5</v>
+        <v>36.1</v>
       </c>
       <c r="S18" s="6">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="T18" s="6" t="s">
         <v>51</v>
@@ -3449,31 +3449,31 @@
         <v>4</v>
       </c>
       <c r="K19" s="6">
-        <v>442.423</v>
+        <v>436.46800000000007</v>
       </c>
       <c r="L19" s="6">
         <v>185</v>
       </c>
       <c r="M19" s="6">
-        <v>36</v>
+        <v>58</v>
       </c>
       <c r="N19" s="6">
-        <v>237.99700000000001</v>
+        <v>152.78499999999974</v>
       </c>
       <c r="O19" s="6">
-        <v>6.6109999999999998</v>
+        <v>3.056</v>
       </c>
       <c r="P19" s="6">
-        <v>27.503</v>
+        <v>13.211000000000013</v>
       </c>
       <c r="Q19" s="6">
-        <v>1.3</v>
+        <v>0.43299999999999272</v>
       </c>
       <c r="R19" s="6">
-        <v>53.8</v>
+        <v>35</v>
       </c>
       <c r="S19" s="6">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="T19" s="6" t="s">
         <v>52</v>
@@ -3514,31 +3514,31 @@
         <v>1</v>
       </c>
       <c r="K20" s="6">
-        <v>230.672</v>
+        <v>229.05300000000005</v>
       </c>
       <c r="L20" s="6">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="M20" s="6">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="N20" s="6">
-        <v>159.446</v>
+        <v>127.07299999999987</v>
       </c>
       <c r="O20" s="6">
-        <v>8.3919999999999995</v>
+        <v>6.0510000000000002</v>
       </c>
       <c r="P20" s="6">
-        <v>26.298999999999999</v>
+        <v>14.572000000000003</v>
       </c>
       <c r="Q20" s="6">
-        <v>2.0230000000000001</v>
+        <v>0.40399999999999636</v>
       </c>
       <c r="R20" s="6">
-        <v>69.099999999999994</v>
+        <v>55.5</v>
       </c>
       <c r="S20" s="6">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="T20" s="6" t="s">
         <v>53</v>
@@ -3579,31 +3579,31 @@
         <v>1</v>
       </c>
       <c r="K21" s="6">
-        <v>236.297</v>
+        <v>227.19399999999996</v>
       </c>
       <c r="L21" s="6">
-        <v>125</v>
+        <v>139</v>
       </c>
       <c r="M21" s="6">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="N21" s="6">
-        <v>150.923</v>
+        <v>123.40800000000013</v>
       </c>
       <c r="O21" s="6">
-        <v>8.3849999999999998</v>
+        <v>7.2590000000000003</v>
       </c>
       <c r="P21" s="6">
-        <v>20.431999999999999</v>
+        <v>18.004999999999995</v>
       </c>
       <c r="Q21" s="6">
-        <v>2.024</v>
+        <v>0.40399999999999636</v>
       </c>
       <c r="R21" s="6">
-        <v>63.9</v>
+        <v>54.3</v>
       </c>
       <c r="S21" s="6">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="T21" s="6" t="s">
         <v>54</v>
@@ -3644,31 +3644,31 @@
         <v>1</v>
       </c>
       <c r="K22" s="6">
-        <v>347.44299999999998</v>
+        <v>346.73500000000001</v>
       </c>
       <c r="L22" s="6">
         <v>207</v>
       </c>
       <c r="M22" s="6">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="N22" s="6">
-        <v>220.4</v>
+        <v>180.65299999999979</v>
       </c>
       <c r="O22" s="6">
-        <v>7.11</v>
+        <v>7.5270000000000001</v>
       </c>
       <c r="P22" s="6">
-        <v>25.893999999999998</v>
+        <v>19.421000000000049</v>
       </c>
       <c r="Q22" s="6">
-        <v>1.0109999999999999</v>
+        <v>0.6069999999999709</v>
       </c>
       <c r="R22" s="6">
-        <v>63.4</v>
+        <v>52.1</v>
       </c>
       <c r="S22" s="6">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="T22" s="6" t="s">
         <v>55</v>
@@ -3709,31 +3709,31 @@
         <v>2</v>
       </c>
       <c r="K23" s="6">
-        <v>233.09899999999999</v>
+        <v>226.22100000000006</v>
       </c>
       <c r="L23" s="6">
         <v>132</v>
       </c>
       <c r="M23" s="6">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="N23" s="6">
-        <v>153.57599999999999</v>
+        <v>116.14200000000011</v>
       </c>
       <c r="O23" s="6">
-        <v>5.4850000000000003</v>
+        <v>4.3019999999999996</v>
       </c>
       <c r="P23" s="6">
-        <v>15.576000000000001</v>
+        <v>9.7100000000000364</v>
       </c>
       <c r="Q23" s="6">
-        <v>1.2150000000000001</v>
+        <v>0.6069999999999709</v>
       </c>
       <c r="R23" s="6">
-        <v>65.900000000000006</v>
+        <v>51.3</v>
       </c>
       <c r="S23" s="6">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="T23" s="6" t="s">
         <v>56</v>
@@ -3774,31 +3774,31 @@
         <v>2</v>
       </c>
       <c r="K24" s="6">
-        <v>240.94800000000001</v>
+        <v>240.54399999999998</v>
       </c>
       <c r="L24" s="6">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="M24" s="6">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="N24" s="6">
-        <v>177.42099999999999</v>
+        <v>116.32499999999993</v>
       </c>
       <c r="O24" s="6">
-        <v>9.8569999999999993</v>
+        <v>4.1539999999999999</v>
       </c>
       <c r="P24" s="6">
-        <v>23.466000000000001</v>
+        <v>13.149000000000001</v>
       </c>
       <c r="Q24" s="6">
-        <v>2.8319999999999999</v>
+        <v>0.20199999999999818</v>
       </c>
       <c r="R24" s="6">
-        <v>73.599999999999994</v>
+        <v>48.4</v>
       </c>
       <c r="S24" s="6">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="T24" s="6" t="s">
         <v>57</v>
@@ -3839,31 +3839,31 @@
         <v>2</v>
       </c>
       <c r="K25" s="6">
-        <v>201.08500000000001</v>
+        <v>198.25299999999993</v>
       </c>
       <c r="L25" s="6">
         <v>103</v>
       </c>
       <c r="M25" s="6">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="N25" s="6">
-        <v>146.666</v>
+        <v>103.37600000000032</v>
       </c>
       <c r="O25" s="6">
-        <v>9.1669999999999998</v>
+        <v>5.1689999999999996</v>
       </c>
       <c r="P25" s="6">
-        <v>29.129000000000001</v>
+        <v>14.36200000000008</v>
       </c>
       <c r="Q25" s="6">
-        <v>1.214</v>
+        <v>0.20300000000020191</v>
       </c>
       <c r="R25" s="6">
-        <v>72.900000000000006</v>
+        <v>52.1</v>
       </c>
       <c r="S25" s="6">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="T25" s="6" t="s">
         <v>58</v>
@@ -3904,31 +3904,31 @@
         <v>1</v>
       </c>
       <c r="K26" s="6">
-        <v>202.548</v>
+        <v>199.298</v>
       </c>
       <c r="L26" s="6">
         <v>178</v>
       </c>
       <c r="M26" s="6">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="N26" s="6">
-        <v>95.314999999999998</v>
+        <v>70.618000000000052</v>
       </c>
       <c r="O26" s="6">
-        <v>5.0170000000000003</v>
+        <v>3.5310000000000001</v>
       </c>
       <c r="P26" s="6">
-        <v>12.131</v>
+        <v>9.964999999999975</v>
       </c>
       <c r="Q26" s="6">
-        <v>1.9490000000000001</v>
+        <v>0.64900000000000091</v>
       </c>
       <c r="R26" s="6">
-        <v>47.1</v>
+        <v>35.4</v>
       </c>
       <c r="S26" s="6">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="T26" s="6" t="s">
         <v>59</v>
@@ -3969,31 +3969,31 @@
         <v>1</v>
       </c>
       <c r="K27" s="6">
-        <v>214.02799999999999</v>
+        <v>213.16199999999992</v>
       </c>
       <c r="L27" s="6">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="M27" s="6">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="N27" s="6">
-        <v>121.31100000000001</v>
+        <v>87.9549999999997</v>
       </c>
       <c r="O27" s="6">
-        <v>7.5819999999999999</v>
+        <v>5.8639999999999999</v>
       </c>
       <c r="P27" s="6">
-        <v>13.430999999999999</v>
+        <v>10.182000000000016</v>
       </c>
       <c r="Q27" s="6">
-        <v>1.2989999999999999</v>
+        <v>0.2159999999998945</v>
       </c>
       <c r="R27" s="6">
-        <v>56.7</v>
+        <v>41.3</v>
       </c>
       <c r="S27" s="6">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="T27" s="6" t="s">
         <v>60</v>
@@ -4034,28 +4034,28 @@
         <v>1</v>
       </c>
       <c r="K28" s="6">
-        <v>262.44299999999998</v>
+        <v>260.60100000000011</v>
       </c>
       <c r="L28" s="6">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="M28" s="6">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="N28" s="6">
-        <v>94.771000000000001</v>
+        <v>61.979000000000724</v>
       </c>
       <c r="O28" s="6">
-        <v>4.9880000000000004</v>
+        <v>4.7679999999999998</v>
       </c>
       <c r="P28" s="6">
-        <v>9.3160000000000007</v>
+        <v>7.1490000000001146</v>
       </c>
       <c r="Q28" s="6">
-        <v>2.6</v>
+        <v>0.21600000000012187</v>
       </c>
       <c r="R28" s="6">
-        <v>36.1</v>
+        <v>23.8</v>
       </c>
       <c r="S28" s="6">
         <v>13</v>
@@ -4099,13 +4099,13 @@
         <v>2</v>
       </c>
       <c r="K29" s="6">
-        <v>7.7980000000000018</v>
+        <v>216.19400000000002</v>
       </c>
       <c r="L29" s="6">
-        <v>-1042</v>
+        <v>168</v>
       </c>
       <c r="M29" s="6">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="N29" s="6">
         <v>91.061000000000263</v>
@@ -4120,7 +4120,7 @@
         <v>0.21699999999998454</v>
       </c>
       <c r="R29" s="6">
-        <v>1167.7</v>
+        <v>42.1</v>
       </c>
       <c r="S29" s="6">
         <v>28</v>
@@ -4164,31 +4164,31 @@
         <v>2</v>
       </c>
       <c r="K30" s="6">
-        <v>232.00700000000001</v>
+        <v>207.74599999999998</v>
       </c>
       <c r="L30" s="6">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="M30" s="6">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="N30" s="6">
-        <v>76.685000000000002</v>
+        <v>55.672000000000025</v>
       </c>
       <c r="O30" s="6">
-        <v>3.8340000000000001</v>
+        <v>3.2749999999999999</v>
       </c>
       <c r="P30" s="6">
-        <v>8.8819999999999997</v>
+        <v>5.6330000000000382</v>
       </c>
       <c r="Q30" s="6">
-        <v>1.7330000000000001</v>
+        <v>0.21600000000000819</v>
       </c>
       <c r="R30" s="6">
-        <v>33.1</v>
+        <v>26.8</v>
       </c>
       <c r="S30" s="6">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="T30" s="6" t="s">
         <v>63</v>
@@ -4229,31 +4229,31 @@
         <v>2</v>
       </c>
       <c r="K31" s="6">
-        <v>232.982</v>
+        <v>232.22400000000005</v>
       </c>
       <c r="L31" s="6">
         <v>85</v>
       </c>
       <c r="M31" s="6">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="N31" s="6">
-        <v>75.164000000000001</v>
+        <v>59.657999999999447</v>
       </c>
       <c r="O31" s="6">
-        <v>4.1760000000000002</v>
+        <v>3.9769999999999999</v>
       </c>
       <c r="P31" s="6">
-        <v>12.997</v>
+        <v>6.7149999999999181</v>
       </c>
       <c r="Q31" s="6">
-        <v>1.083</v>
+        <v>0.21699999999987085</v>
       </c>
       <c r="R31" s="6">
-        <v>32.299999999999997</v>
+        <v>25.7</v>
       </c>
       <c r="S31" s="6">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="T31" s="6" t="s">
         <v>64</v>
@@ -4330,5 +4330,6 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
enlever le couvert n'est plus une bouchée
</commit_message>
<xml_diff>
--- a/Resultats exp bag_couverts/Resultats exp bag_couverts/Tableau récapitulatif - new algo.xlsx
+++ b/Resultats exp bag_couverts/Resultats exp bag_couverts/Tableau récapitulatif - new algo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abarb\Documents\travail\stage et4\travail\codePlateau\Resultats exp bag_couverts\Resultats exp bag_couverts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A72450A-11C7-4A8C-AF00-2CEE94F123A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDA7276C-9D28-4361-90E0-A42C96B65260}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="11625" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2254,10 +2254,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A472D21A-79DB-4329-B4B1-053817E0ED03}">
-  <dimension ref="A1:U32"/>
+  <dimension ref="A1:U41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD10"/>
+      <selection activeCell="G11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2929,19 +2929,19 @@
         <v>2</v>
       </c>
       <c r="K11" s="6">
-        <v>262.46799999999996</v>
+        <v>247.09199999999998</v>
       </c>
       <c r="L11" s="6">
-        <v>146</v>
+        <v>132</v>
       </c>
       <c r="M11" s="6">
         <v>31</v>
       </c>
       <c r="N11" s="6">
-        <v>106.54500000000004</v>
+        <v>106.76200000000003</v>
       </c>
       <c r="O11" s="6">
-        <v>4.843</v>
+        <v>5.6189999999999998</v>
       </c>
       <c r="P11" s="6">
         <v>8.4449999999999932</v>
@@ -2950,10 +2950,10 @@
         <v>0.21600000000000819</v>
       </c>
       <c r="R11" s="6">
-        <v>40.6</v>
+        <v>43.2</v>
       </c>
       <c r="S11" s="6">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="T11" s="6" t="s">
         <v>44</v>
@@ -4325,6 +4325,47 @@
       </c>
       <c r="U32" s="6" t="s">
         <v>70</v>
+      </c>
+    </row>
+    <row r="37" spans="13:18" x14ac:dyDescent="0.45">
+      <c r="Q37">
+        <v>146</v>
+      </c>
+      <c r="R37">
+        <f>753-635</f>
+        <v>118</v>
+      </c>
+    </row>
+    <row r="38" spans="13:18" x14ac:dyDescent="0.45">
+      <c r="M38">
+        <f>876-869</f>
+        <v>7</v>
+      </c>
+      <c r="Q38">
+        <v>113</v>
+      </c>
+      <c r="R38">
+        <f>876-756</f>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="39" spans="13:18" x14ac:dyDescent="0.45">
+      <c r="Q39">
+        <v>118</v>
+      </c>
+      <c r="R39">
+        <f>964-832</f>
+        <v>132</v>
+      </c>
+    </row>
+    <row r="41" spans="13:18" x14ac:dyDescent="0.45">
+      <c r="Q41">
+        <f>SUM(Q37:Q39)</f>
+        <v>377</v>
+      </c>
+      <c r="R41">
+        <f>SUM(R37:R39)</f>
+        <v>370</v>
       </c>
     </row>
   </sheetData>

</xml_diff>